<commit_message>
IF-123 update oracle integration
</commit_message>
<xml_diff>
--- a/Integration Hub.xlsx
+++ b/Integration Hub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Integration_Hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16253F27-5FEF-4FEB-BCF2-37DF42CDCB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143160C0-9F64-4281-8E36-6DBFC2E2D3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6F717C97-0D54-4045-BCFD-B0769D55B9C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{6F717C97-0D54-4045-BCFD-B0769D55B9C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Integrations" sheetId="11" r:id="rId1"/>
@@ -528,9 +528,6 @@
     <t>https://documents.bmc.com/supportu/9.0.21.300/en-US/Documentation/OCI_VM.htm</t>
   </si>
   <si>
-    <t>https://documents.bmc.com/supportu/9.0.21.300/en-US/Documentation/ODI_Data_Flow.htm</t>
-  </si>
-  <si>
     <t>https://documents.bmc.com/supportu/9.0.21.300/en-US/Documentation/Openshift_Kubernetes.htm</t>
   </si>
   <si>
@@ -780,9 +777,6 @@
     <t>https://github.com/BMCDBA/oci_vm</t>
   </si>
   <si>
-    <t>https://github.com/BMCDBA/odi_data_flow</t>
-  </si>
-  <si>
     <t>https://github.com/BMCDBA/openshift_kubernetes</t>
   </si>
   <si>
@@ -1099,6 +1093,12 @@
   </si>
   <si>
     <t>https://docs.oracle.com/en-us/iaas/releasenotes/services/compute/</t>
+  </si>
+  <si>
+    <t>https://documents.bmc.com/supportu/9.0.21.300/en-US/Documentation/OCI_Data_Flow.htm</t>
+  </si>
+  <si>
+    <t>https://github.com/BMCDBA/oci_data_flow</t>
   </si>
 </sst>
 </file>
@@ -2527,8 +2527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB88ED17-33F3-4CCE-9713-B47C5FAF7F78}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,10 +2548,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>91</v>
@@ -2565,13 +2565,13 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>92</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2582,30 +2582,30 @@
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2616,13 +2616,13 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2633,13 +2633,13 @@
         <v>79</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>95</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2650,13 +2650,13 @@
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2667,13 +2667,13 @@
         <v>79</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>97</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2684,13 +2684,13 @@
         <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>135</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2701,13 +2701,13 @@
         <v>78</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>136</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2718,13 +2718,13 @@
         <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>125</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2735,13 +2735,13 @@
         <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>137</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2752,13 +2752,13 @@
         <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>138</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2769,13 +2769,13 @@
         <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>152</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2786,13 +2786,13 @@
         <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>153</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2803,13 +2803,13 @@
         <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>154</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2820,13 +2820,13 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>155</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2837,13 +2837,13 @@
         <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>156</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2854,13 +2854,13 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>157</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2871,13 +2871,13 @@
         <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2888,13 +2888,13 @@
         <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2905,13 +2905,13 @@
         <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2922,13 +2922,13 @@
         <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2939,13 +2939,13 @@
         <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2956,13 +2956,13 @@
         <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2973,13 +2973,13 @@
         <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2990,13 +2990,13 @@
         <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3007,13 +3007,13 @@
         <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3024,13 +3024,13 @@
         <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3041,13 +3041,13 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3069,7 +3069,7 @@
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="97" customWidth="1"/>
+    <col min="3" max="3" width="82.42578125" customWidth="1"/>
     <col min="4" max="4" width="97.7109375" customWidth="1"/>
     <col min="5" max="5" width="49.5703125" customWidth="1"/>
   </cols>
@@ -3082,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>91</v>
@@ -3099,13 +3099,13 @@
         <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>98</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3116,13 +3116,13 @@
         <v>78</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>99</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3133,13 +3133,13 @@
         <v>76</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>100</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3150,13 +3150,13 @@
         <v>79</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>101</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3167,13 +3167,13 @@
         <v>80</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>102</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3184,13 +3184,13 @@
         <v>78</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>103</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3201,13 +3201,13 @@
         <v>78</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3218,13 +3218,13 @@
         <v>78</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>105</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3235,13 +3235,13 @@
         <v>79</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>106</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3252,13 +3252,13 @@
         <v>81</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>107</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3269,13 +3269,13 @@
         <v>77</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>108</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3286,13 +3286,13 @@
         <v>76</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>109</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3303,13 +3303,13 @@
         <v>82</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>110</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3320,13 +3320,13 @@
         <v>78</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>111</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3337,13 +3337,13 @@
         <v>80</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>112</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3354,13 +3354,13 @@
         <v>78</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>113</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3371,13 +3371,13 @@
         <v>77</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>114</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3388,13 +3388,13 @@
         <v>77</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>115</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3405,13 +3405,13 @@
         <v>76</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>116</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3422,13 +3422,13 @@
         <v>78</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>117</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3439,13 +3439,13 @@
         <v>77</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>118</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3456,13 +3456,13 @@
         <v>77</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>119</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3473,13 +3473,13 @@
         <v>76</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>120</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3784,10 +3784,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>91</v>
@@ -3801,13 +3801,13 @@
         <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>121</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3818,13 +3818,13 @@
         <v>80</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>122</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3835,13 +3835,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>123</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3852,30 +3852,30 @@
         <v>83</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>124</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3886,13 +3886,13 @@
         <v>76</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>126</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3903,13 +3903,13 @@
         <v>81</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>127</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3920,13 +3920,13 @@
         <v>78</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>128</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3937,13 +3937,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>129</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3954,13 +3954,13 @@
         <v>78</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>130</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3971,13 +3971,13 @@
         <v>78</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>131</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3988,13 +3988,13 @@
         <v>76</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>132</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4005,13 +4005,13 @@
         <v>80</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>133</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4022,13 +4022,13 @@
         <v>81</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>134</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4067,10 +4067,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>91</v>
@@ -4084,13 +4084,13 @@
         <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4101,13 +4101,13 @@
         <v>79</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>140</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4118,13 +4118,13 @@
         <v>79</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>141</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4135,13 +4135,13 @@
         <v>77</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>142</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4152,13 +4152,13 @@
         <v>77</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>143</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4169,13 +4169,13 @@
         <v>81</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>144</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4186,13 +4186,13 @@
         <v>78</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4203,13 +4203,13 @@
         <v>78</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>146</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4220,13 +4220,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>147</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4237,13 +4237,13 @@
         <v>78</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>148</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4254,13 +4254,13 @@
         <v>81</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>149</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4271,13 +4271,13 @@
         <v>81</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>150</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4288,13 +4288,13 @@
         <v>76</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>151</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4309,8 +4309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5C4FDE-C3C6-4FF2-B593-07C4096B3434}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4331,10 +4331,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>91</v>
@@ -4342,94 +4342,97 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>81</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>246</v>
+        <v>351</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>158</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>159</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>160</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>161</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B077FD2C-916C-46DA-A33F-5461EDA59CF1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IF-123 fix: Fix integration card layout issue
</commit_message>
<xml_diff>
--- a/Integration Hub.xlsx
+++ b/Integration Hub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Integration_Hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911B7756-563B-4286-92C1-AE8AD914393F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BEB3CE-B70C-4673-8175-B969C8C1EBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6F717C97-0D54-4045-BCFD-B0769D55B9C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6F717C97-0D54-4045-BCFD-B0769D55B9C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Integrations" sheetId="11" r:id="rId1"/>
@@ -315,6 +315,9 @@
     <t>IBM Datastage</t>
   </si>
   <si>
+    <t>Documentation URL</t>
+  </si>
+  <si>
     <t>https://documents.bmc.com/supportu/9.0.21.300/en-US/Documentation/Airbyte.htm</t>
   </si>
   <si>
@@ -924,9 +927,6 @@
     <t>https://docs.vmware.com/en/VMware-vSphere/index.html</t>
   </si>
   <si>
-    <t>Release Notes URL</t>
-  </si>
-  <si>
     <t>https://docs.aws.amazon.com/apprunner/latest/relnotes/relnotes.html</t>
   </si>
   <si>
@@ -1350,10 +1350,10 @@
     <t>https://developer.vmware.com/</t>
   </si>
   <si>
-    <t>GitHub Repository URL</t>
-  </si>
-  <si>
-    <t>ControlM Documentation URL</t>
+    <t>GitHub  URL</t>
+  </si>
+  <si>
+    <t>ControlM Doc URL</t>
   </si>
 </sst>
 </file>
@@ -1565,11 +1565,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1583,7 +1584,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1599,7 +1599,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2863,9 +2862,9 @@
     <tableColumn id="1" xr3:uid="{681642ED-3CD9-41E8-B36B-A5951755DAED}" name="Integration Name" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{27758331-E9B0-46BB-A800-ED6BE796FC0A}" name="Developer" dataDxfId="15"/>
     <tableColumn id="7" xr3:uid="{480B3A6A-24A6-45D5-87B3-938863E4D3BB}" name="API Documentation URL" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{1DE41592-E13D-4FC9-BFDA-AC6BE0FD6339}" name="Release Notes URL" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{2C1AB673-125A-416A-ABA9-FA9A326D97F7}" name="ControlM Documentation URL" dataDxfId="12" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{1B934557-DB41-4222-9E0B-20F8B9383FC0}" name="GitHub Repository URL" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{1DE41592-E13D-4FC9-BFDA-AC6BE0FD6339}" name="Documentation URL" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{2C1AB673-125A-416A-ABA9-FA9A326D97F7}" name="ControlM Doc URL" dataDxfId="12" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{1B934557-DB41-4222-9E0B-20F8B9383FC0}" name="GitHub  URL" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2881,9 +2880,9 @@
     <tableColumn id="1" xr3:uid="{1A67D51F-7022-4A5B-BDCC-B0E728C261E6}" name="Integration Name" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{23F091F4-53F1-484C-BDC1-1E37F4AFCDFE}" name="Developer" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{232EEDCC-1A87-4915-A6E5-85A79E2BB17B}" name="API Documentation URL" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E8756A58-C5B5-41D2-9EE8-B8B43D50FB22}" name="Release Notes URL" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{80F5DF6A-C464-48E8-82AB-99C1FEA65D5C}" name="ControlM Documentation URL" dataDxfId="2" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{F9330334-ABAE-42A8-B738-364C05F78089}" name="GitHub Repository URL" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{E8756A58-C5B5-41D2-9EE8-B8B43D50FB22}" name="Documentation URL" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{80F5DF6A-C464-48E8-82AB-99C1FEA65D5C}" name="ControlM Doc URL" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{F9330334-ABAE-42A8-B738-364C05F78089}" name="GitHub  URL" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2899,9 +2898,9 @@
     <tableColumn id="1" xr3:uid="{80D381EF-AD46-4F3A-BBFF-8DBB1B438E51}" name="Integration Name" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{6E53A2E0-1374-4099-911C-E7602B04F2DB}" name="Developer" dataDxfId="28"/>
     <tableColumn id="6" xr3:uid="{DDEA3AF2-E27C-4DC3-8901-B80C18040A41}" name="API Documentation URL" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{D6E3BA2B-8418-46C4-9A7F-4F7D1974CB48}" name="Release Notes URL" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{7ABCE907-A038-489C-9A89-61BB2338F1FA}" name="ControlM Documentation URL" dataDxfId="25" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{E0C91B3B-110A-43F6-B19A-2CD2143B502D}" name="GitHub Repository URL" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{D6E3BA2B-8418-46C4-9A7F-4F7D1974CB48}" name="Documentation URL" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{7ABCE907-A038-489C-9A89-61BB2338F1FA}" name="ControlM Doc URL" dataDxfId="25" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{E0C91B3B-110A-43F6-B19A-2CD2143B502D}" name="GitHub  URL" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2917,9 +2916,9 @@
     <tableColumn id="1" xr3:uid="{EE328544-C28B-44E7-A75D-0369A6EA4CB7}" name="Integration Name" dataDxfId="37"/>
     <tableColumn id="2" xr3:uid="{21843E6B-EF24-4884-B1BF-0ECCC9A28A99}" name="Developer" dataDxfId="36"/>
     <tableColumn id="6" xr3:uid="{06EA03F2-4673-45FE-8868-395780C8A90C}" name="API Documentation URL" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{9EC64632-4A20-458E-B708-20C81D7E40C6}" name="Release Notes URL" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{3420A52B-DE89-4C17-A876-7D15E7EB436D}" name="ControlM Documentation URL" dataDxfId="33" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{6CD5348A-5EE8-4424-A4D1-87D1FCAF47A5}" name="GitHub Repository URL" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{9EC64632-4A20-458E-B708-20C81D7E40C6}" name="Documentation URL" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{3420A52B-DE89-4C17-A876-7D15E7EB436D}" name="ControlM Doc URL" dataDxfId="33" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{6CD5348A-5EE8-4424-A4D1-87D1FCAF47A5}" name="GitHub  URL" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2935,9 +2934,9 @@
     <tableColumn id="1" xr3:uid="{B36A509B-FEE8-4F41-941B-FF0512867FA8}" name="Integration Name" dataDxfId="45"/>
     <tableColumn id="2" xr3:uid="{BAFC04A2-C75E-49DB-9355-1C3AD10F7A4A}" name="Developer" dataDxfId="44"/>
     <tableColumn id="6" xr3:uid="{5C687AFF-5F82-4441-AFF5-0C1191ABC593}" name="API Documentation URL" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{C66AA305-53A0-4703-AAF1-894DBD4A7BD7}" name="Release Notes URL" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{6E890E5B-193A-4D96-ACA6-7D0681B3640B}" name="ControlM Documentation URL" dataDxfId="41" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{BE6C341D-AA8F-46C2-840F-45E7E16F269B}" name="GitHub Repository URL" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{C66AA305-53A0-4703-AAF1-894DBD4A7BD7}" name="Documentation URL" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{6E890E5B-193A-4D96-ACA6-7D0681B3640B}" name="ControlM Doc URL" dataDxfId="41" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{BE6C341D-AA8F-46C2-840F-45E7E16F269B}" name="GitHub  URL" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3262,35 +3261,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB88ED17-33F3-4CCE-9713-B47C5FAF7F78}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C30"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F1" sqref="C1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76" style="5" customWidth="1"/>
-    <col min="4" max="4" width="71" style="5" customWidth="1"/>
-    <col min="5" max="5" width="101.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="18.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76" style="6" customWidth="1"/>
+    <col min="4" max="4" width="71" style="6" customWidth="1"/>
+    <col min="5" max="5" width="101.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>437</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -3298,563 +3297,563 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>407</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>91</v>
+        <v>266</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="F4" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="C10" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="8" t="s">
         <v>434</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>170</v>
+        <v>293</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3868,13 +3867,13 @@
         <v>435</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3890,35 +3889,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B82786-371F-425B-948D-AB2F7BB6D165}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="72.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="77.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="24.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="72.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="77.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>437</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -3926,443 +3925,443 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>97</v>
+      <c r="E2" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>98</v>
+      <c r="E3" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>99</v>
+      <c r="E4" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>100</v>
+      <c r="E5" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>101</v>
+      <c r="E6" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>102</v>
+      <c r="E7" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>103</v>
+      <c r="E8" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>104</v>
+      <c r="E9" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>105</v>
+      <c r="E10" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>106</v>
+      <c r="E11" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>107</v>
+      <c r="E12" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>108</v>
+      <c r="E13" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>109</v>
+      <c r="E14" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>110</v>
+      <c r="E15" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>111</v>
+      <c r="E16" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>112</v>
+      <c r="E17" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>113</v>
+      <c r="E18" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>114</v>
+      <c r="E19" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>115</v>
+      <c r="E20" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>116</v>
+      <c r="E21" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>117</v>
+      <c r="E22" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>118</v>
+      <c r="E23" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4379,10 +4378,10 @@
         <v>317</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4722,35 +4721,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A28C5E4-4B1E-4221-AC99-B3F344F7E1EF}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20" style="5" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="80" style="5" customWidth="1"/>
-    <col min="6" max="6" width="40.42578125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="22.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20" style="6" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="80" style="6" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>437</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -4758,263 +4757,263 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>120</v>
+      <c r="E2" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>121</v>
+      <c r="E3" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>122</v>
+      <c r="E4" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>123</v>
+      <c r="E5" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>257</v>
+      <c r="E6" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>125</v>
+      <c r="E7" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>126</v>
+      <c r="E8" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>127</v>
+      <c r="E9" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>128</v>
+      <c r="E10" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>129</v>
+      <c r="E11" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>130</v>
+      <c r="E12" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>131</v>
+      <c r="E13" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>132</v>
+      <c r="E14" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5030,11 +5029,11 @@
       <c r="D15" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>133</v>
+      <c r="E15" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -5051,34 +5050,34 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="79.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="49.7109375" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="22.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="79.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>437</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -5086,243 +5085,243 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>138</v>
+      <c r="E2" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>139</v>
+      <c r="E3" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>140</v>
+      <c r="E4" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>141</v>
+      <c r="E5" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>142</v>
+      <c r="E6" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>143</v>
+      <c r="E7" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>144</v>
+      <c r="E8" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>145</v>
+      <c r="E9" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>146</v>
+      <c r="E10" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>147</v>
+      <c r="E11" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>148</v>
+      <c r="E12" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>149</v>
+      <c r="E13" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5338,22 +5337,18 @@
       <c r="D14" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>150</v>
+      <c r="E14" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{28C6D50A-C1CC-4CE4-BB96-EF2A14B8B10F}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{D28C5F8D-63DD-44FD-AD37-45FC269242C4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5368,31 +5363,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="56" style="5" customWidth="1"/>
-    <col min="5" max="5" width="77.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="5"/>
-    <col min="9" max="9" width="9.42578125" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="24.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="56" style="6" customWidth="1"/>
+    <col min="5" max="5" width="77.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="6"/>
+    <col min="9" max="9" width="9.42578125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>437</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -5400,88 +5395,88 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="2" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>157</v>
+      <c r="E3" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>158</v>
+      <c r="E4" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>159</v>
+      <c r="E5" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>78</v>
@@ -5492,21 +5487,18 @@
       <c r="D6" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>160</v>
+      <c r="E6" s="9" t="s">
+        <v>161</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{B077FD2C-916C-46DA-A33F-5461EDA59CF1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>